<commit_message>
made no X and IL version of TW db
</commit_message>
<xml_diff>
--- a/analyses/unipept/lca/T12_325_digested_PeaksDB_lca-mc.xlsx
+++ b/analyses/unipept/lca/T12_325_digested_PeaksDB_lca-mc.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="T12_325_digested_PeaksDB_lca-mc" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="diatom only" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="diatom chloroplast protein name" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="1295">
   <si>
     <t xml:space="preserve">peptide</t>
   </si>
@@ -3857,6 +3859,54 @@
   </si>
   <si>
     <t xml:space="preserve">NEADMLDLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database protein ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0171421366 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201829098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201860448 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203152572 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203172898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203203762 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203226722 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203265014 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203358160 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203473996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203508352 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKF1|A0A089VKF1_THAWE ATP synthase subunit c, chloroplastic OS=Thalassiosira weissflogii OX=1577725 GN=atpH PE=3 SV=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKJ4|A0A089VKJ4_THAWE Photosystem I reaction center subunit XI OS=Thalassiosira weissflogii OX=1577725 GN=psaL PE=3 SV=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VP78|A0A089VP78_THAWE Photosystem II reaction center protein Z OS=Thalassiosira weissflogii OX=1577725 GN=psbZ PE=3 SV=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|O96712|O96712_THAWE Fucoxanthin chlorophyll a/c binding protein (Fragment) OS=Thalassiosira weissflogii OX=1577725 GN=FCP PE=4 SV=1</t>
   </si>
 </sst>
 </file>
@@ -3930,8 +3980,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3954,8 +4008,8 @@
   </sheetPr>
   <dimension ref="A1:AW286"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH27" activeCellId="0" sqref="AH27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10189,4 +10243,1630 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AT23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="41.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP2" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP3" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP4" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI5" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP5" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP6" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO7" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP7" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP8" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL9" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="AM9" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="AN9" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="AO9" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="AP9" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ11" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK11" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL11" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM11" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO11" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP11" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK12" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM12" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN12" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP12" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ13" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK13" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL13" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN13" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP13" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="AG14" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="AK14" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL14" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="AM14" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="AN14" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="AO14" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="AP14" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ14" s="0" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG15" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="AH15" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="AI15" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="AJ15" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="AK15" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="AL15" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="AM15" s="0" t="s">
+        <v>645</v>
+      </c>
+      <c r="AN15" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="AO15" s="0" t="s">
+        <v>647</v>
+      </c>
+      <c r="AP15" s="0" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG16" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="AH16" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="AK16" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="AL16" s="0" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W17" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA17" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="AG17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ17" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP17" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>875</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="AG18" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="AH18" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="AI18" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="AJ18" s="0" t="s">
+        <v>881</v>
+      </c>
+      <c r="AK18" s="0" t="s">
+        <v>882</v>
+      </c>
+      <c r="AL18" s="0" t="s">
+        <v>883</v>
+      </c>
+      <c r="AM18" s="0" t="s">
+        <v>884</v>
+      </c>
+      <c r="AN18" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="AO18" s="0" t="s">
+        <v>886</v>
+      </c>
+      <c r="AP18" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="AQ18" s="0" t="s">
+        <v>888</v>
+      </c>
+      <c r="AR18" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="AS18" s="0" t="s">
+        <v>889</v>
+      </c>
+      <c r="AT18" s="0" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>917</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI19" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="AJ19" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="AK19" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="AL19" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AM19" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AN19" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="AO19" s="0" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI20" s="0" t="s">
+        <v>992</v>
+      </c>
+      <c r="AJ20" s="0" t="s">
+        <v>993</v>
+      </c>
+      <c r="AK20" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="AL20" s="0" t="s">
+        <v>995</v>
+      </c>
+      <c r="AM20" s="0" t="s">
+        <v>996</v>
+      </c>
+      <c r="AN20" s="0" t="s">
+        <v>997</v>
+      </c>
+      <c r="AO20" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="AP20" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="AQ20" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="AR20" s="0" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="AA21" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="AG21" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="AH21" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="AK21" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL21" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG22" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="AH22" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="AI22" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="AJ22" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="AK22" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="AL22" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="AM22" s="0" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="W23" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE23" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AF23" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AI23" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AJ23" s="0" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AK23" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AL23" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="AM23" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="AN23" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="AO23" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AP23" s="0" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>